<commit_message>
Final commit for assignment 3
</commit_message>
<xml_diff>
--- a/Assignment 3/results/heatMap.xlsx
+++ b/Assignment 3/results/heatMap.xlsx
@@ -1,24 +1,262 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="21075" windowHeight="9030"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="21080" windowHeight="9040"/>
   </bookViews>
   <sheets>
     <sheet name="heatMap" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
+  <si>
+    <t>2.0.2.5</t>
+  </si>
+  <si>
+    <t>2.0.2.6</t>
+  </si>
+  <si>
+    <t>2.0.2.7</t>
+  </si>
+  <si>
+    <t>2.0.3.0</t>
+  </si>
+  <si>
+    <t>2.0.3.2</t>
+  </si>
+  <si>
+    <t>2.0.4.0</t>
+  </si>
+  <si>
+    <t>2.0.4.2</t>
+  </si>
+  <si>
+    <t>2.0.6.0</t>
+  </si>
+  <si>
+    <t>2.0.7.0</t>
+  </si>
+  <si>
+    <t>2.0.8.0</t>
+  </si>
+  <si>
+    <t>2.0.8.2</t>
+  </si>
+  <si>
+    <t>2.0.8.4</t>
+  </si>
+  <si>
+    <t>2.1.0.0</t>
+  </si>
+  <si>
+    <t>2.1.0.2</t>
+  </si>
+  <si>
+    <t>2.1.0.4</t>
+  </si>
+  <si>
+    <t>2.2.0.0</t>
+  </si>
+  <si>
+    <t>2.2.0.2</t>
+  </si>
+  <si>
+    <t>2.3.0.0</t>
+  </si>
+  <si>
+    <t>2.3.0.2</t>
+  </si>
+  <si>
+    <t>2.3.0.4</t>
+  </si>
+  <si>
+    <t>2.3.0.6</t>
+  </si>
+  <si>
+    <t>2.4.0.0</t>
+  </si>
+  <si>
+    <t>2.4.0.2</t>
+  </si>
+  <si>
+    <t>2.5.0.0</t>
+  </si>
+  <si>
+    <t>2.5.0.2</t>
+  </si>
+  <si>
+    <t>2.5.0.4</t>
+  </si>
+  <si>
+    <t>3.0.0.6</t>
+  </si>
+  <si>
+    <t>3.0.0.8</t>
+  </si>
+  <si>
+    <t>3.0.1.0</t>
+  </si>
+  <si>
+    <t>3.0.1.2</t>
+  </si>
+  <si>
+    <t>3.0.1.4</t>
+  </si>
+  <si>
+    <t>3.0.1.6</t>
+  </si>
+  <si>
+    <t>3.0.2.0</t>
+  </si>
+  <si>
+    <t>3.0.2.2</t>
+  </si>
+  <si>
+    <t>3.0.3.0</t>
+  </si>
+  <si>
+    <t>3.0.3.4</t>
+  </si>
+  <si>
+    <t>3.0.4.0</t>
+  </si>
+  <si>
+    <t>3.0.4.2</t>
+  </si>
+  <si>
+    <t>3.0.5.0</t>
+  </si>
+  <si>
+    <t>3.0.5.2</t>
+  </si>
+  <si>
+    <t>3.1.0.0</t>
+  </si>
+  <si>
+    <t>3.1.1.0</t>
+  </si>
+  <si>
+    <t>4.0.0.0</t>
+  </si>
+  <si>
+    <t>4.0.0.2</t>
+  </si>
+  <si>
+    <t>4.0.0.4</t>
+  </si>
+  <si>
+    <t>4.1.0.0</t>
+  </si>
+  <si>
+    <t>4.1.0.2</t>
+  </si>
+  <si>
+    <t>4.1.0.4</t>
+  </si>
+  <si>
+    <t>4.2.0.0</t>
+  </si>
+  <si>
+    <t>4.2.0.2</t>
+  </si>
+  <si>
+    <t>4.2.0.4</t>
+  </si>
+  <si>
+    <t>4.2.0.8</t>
+  </si>
+  <si>
+    <t>4.3.0.0</t>
+  </si>
+  <si>
+    <t>4.3.0.2</t>
+  </si>
+  <si>
+    <t>4.3.0.4</t>
+  </si>
+  <si>
+    <t>4.3.0.6</t>
+  </si>
+  <si>
+    <t>4.3.1.0</t>
+  </si>
+  <si>
+    <t>4.3.1.2</t>
+  </si>
+  <si>
+    <t>4.3.1.4</t>
+  </si>
+  <si>
+    <t>4.4.0.0</t>
+  </si>
+  <si>
+    <t>4.4.0.2</t>
+  </si>
+  <si>
+    <t>4.4.0.4</t>
+  </si>
+  <si>
+    <t>4.4.0.6</t>
+  </si>
+  <si>
+    <t>4.4.1.0</t>
+  </si>
+  <si>
+    <t>4.5.0.0</t>
+  </si>
+  <si>
+    <t>4.5.0.2</t>
+  </si>
+  <si>
+    <t>4.5.0.4</t>
+  </si>
+  <si>
+    <t>4.5.1.0</t>
+  </si>
+  <si>
+    <t>4.6.0.0</t>
+  </si>
+  <si>
+    <t>4.6.0.2</t>
+  </si>
+  <si>
+    <t>4.6.0.4</t>
+  </si>
+  <si>
+    <t>4.7.0.0</t>
+  </si>
+  <si>
+    <t>4.7.0.2</t>
+  </si>
+  <si>
+    <t>4.7.1.0</t>
+  </si>
+  <si>
+    <t>2.0.0.8</t>
+  </si>
+  <si>
+    <t>2.0.1.0</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode=";;;"/>
+    <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +395,28 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,7 +719,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -502,10 +762,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
@@ -517,7 +781,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -546,11 +810,15 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -860,17 +1128,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G55" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="O59" sqref="O59"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5" customWidth="1"/>
-    <col min="2" max="75" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="5" customWidth="1"/>
+    <col min="2" max="75" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75">
       <c r="A1" s="4"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -947,7 +1215,7 @@
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75">
       <c r="A2" s="4"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1024,9 +1292,9 @@
       <c r="BV2" s="1"/>
       <c r="BW2" s="1"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2025</v>
+    <row r="3" spans="1:75">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>0.254030016676</v>
@@ -1105,9 +1373,9 @@
       <c r="BV3" s="1"/>
       <c r="BW3" s="1"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2026</v>
+    <row r="4" spans="1:75">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>0.26241448555199998</v>
@@ -1188,9 +1456,9 @@
       <c r="BV4" s="1"/>
       <c r="BW4" s="1"/>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>2027</v>
+    <row r="5" spans="1:75">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="B5" s="1">
         <v>0.244036330971</v>
@@ -1273,9 +1541,9 @@
       <c r="BV5" s="1"/>
       <c r="BW5" s="1"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>2030</v>
+    <row r="6" spans="1:75">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>0.19970189112799999</v>
@@ -1360,9 +1628,9 @@
       <c r="BV6" s="1"/>
       <c r="BW6" s="1"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>2032</v>
+    <row r="7" spans="1:75">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>0.141041292639</v>
@@ -1449,9 +1717,9 @@
       <c r="BV7" s="1"/>
       <c r="BW7" s="1"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>2040</v>
+    <row r="8" spans="1:75">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>7.83277018155E-2</v>
@@ -1540,9 +1808,9 @@
       <c r="BV8" s="1"/>
       <c r="BW8" s="1"/>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>2042</v>
+    <row r="9" spans="1:75">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>7.8816295685600002E-2</v>
@@ -1633,9 +1901,9 @@
       <c r="BV9" s="1"/>
       <c r="BW9" s="1"/>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>2060</v>
+    <row r="10" spans="1:75">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B10" s="1">
         <v>4.1422008205799998E-2</v>
@@ -1728,9 +1996,9 @@
       <c r="BV10" s="1"/>
       <c r="BW10" s="1"/>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>2070</v>
+    <row r="11" spans="1:75">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>3.10552300187E-2</v>
@@ -1825,9 +2093,9 @@
       <c r="BV11" s="1"/>
       <c r="BW11" s="1"/>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>2080</v>
+    <row r="12" spans="1:75">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>2.2279586285799999E-2</v>
@@ -1924,9 +2192,9 @@
       <c r="BV12" s="1"/>
       <c r="BW12" s="1"/>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>2082</v>
+    <row r="13" spans="1:75">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>2.1298528697599999E-2</v>
@@ -2025,9 +2293,9 @@
       <c r="BV13" s="1"/>
       <c r="BW13" s="1"/>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>2084</v>
+    <row r="14" spans="1:75">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B14" s="1">
         <v>1.9941610963100001E-2</v>
@@ -2128,9 +2396,9 @@
       <c r="BV14" s="1"/>
       <c r="BW14" s="1"/>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>2100</v>
+    <row r="15" spans="1:75">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B15" s="1">
         <v>1.19224225927E-2</v>
@@ -2233,9 +2501,9 @@
       <c r="BV15" s="1"/>
       <c r="BW15" s="1"/>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>2102</v>
+    <row r="16" spans="1:75">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>9.08199968187E-3</v>
@@ -2340,9 +2608,9 @@
       <c r="BV16" s="1"/>
       <c r="BW16" s="1"/>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>2104</v>
+    <row r="17" spans="1:75">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>8.6401070774000006E-3</v>
@@ -2449,9 +2717,9 @@
       <c r="BV17" s="1"/>
       <c r="BW17" s="1"/>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>2200</v>
+    <row r="18" spans="1:75">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>5.3300675955400001E-3</v>
@@ -2560,9 +2828,9 @@
       <c r="BV18" s="1"/>
       <c r="BW18" s="1"/>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>2202</v>
+    <row r="19" spans="1:75">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>4.5531994684500001E-3</v>
@@ -2673,9 +2941,9 @@
       <c r="BV19" s="1"/>
       <c r="BW19" s="1"/>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>2300</v>
+    <row r="20" spans="1:75">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B20" s="1">
         <v>3.2658234018200002E-3</v>
@@ -2788,9 +3056,9 @@
       <c r="BV20" s="1"/>
       <c r="BW20" s="1"/>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>2302</v>
+    <row r="21" spans="1:75">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B21" s="1">
         <v>3.1010267643899999E-3</v>
@@ -2905,9 +3173,9 @@
       <c r="BV21" s="1"/>
       <c r="BW21" s="1"/>
     </row>
-    <row r="22" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>2304</v>
+    <row r="22" spans="1:75">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B22" s="1">
         <v>3.0107047279200002E-3</v>
@@ -3024,9 +3292,9 @@
       <c r="BV22" s="1"/>
       <c r="BW22" s="1"/>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>2306</v>
+    <row r="23" spans="1:75">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>2.6358520991000001E-3</v>
@@ -3145,9 +3413,9 @@
       <c r="BV23" s="1"/>
       <c r="BW23" s="1"/>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>2400</v>
+    <row r="24" spans="1:75">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B24" s="1">
         <v>1.84254734076E-3</v>
@@ -3268,9 +3536,9 @@
       <c r="BV24" s="1"/>
       <c r="BW24" s="1"/>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>2402</v>
+    <row r="25" spans="1:75">
+      <c r="A25" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B25" s="1">
         <v>1.8598642843799999E-3</v>
@@ -3393,9 +3661,9 @@
       <c r="BV25" s="1"/>
       <c r="BW25" s="1"/>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>2500</v>
+    <row r="26" spans="1:75">
+      <c r="A26" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B26" s="1">
         <v>1.51796142907E-3</v>
@@ -3520,9 +3788,9 @@
       <c r="BV26" s="1"/>
       <c r="BW26" s="1"/>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>2502</v>
+    <row r="27" spans="1:75">
+      <c r="A27" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B27" s="1">
         <v>1.3110603322899999E-3</v>
@@ -3649,9 +3917,9 @@
       <c r="BV27" s="1"/>
       <c r="BW27" s="1"/>
     </row>
-    <row r="28" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>2504</v>
+    <row r="28" spans="1:75">
+      <c r="A28" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B28" s="1">
         <v>1.2957456675300001E-3</v>
@@ -3780,9 +4048,9 @@
       <c r="BV28" s="1"/>
       <c r="BW28" s="1"/>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>3006</v>
+    <row r="29" spans="1:75">
+      <c r="A29" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B29" s="1">
         <v>1.2957456675300001E-3</v>
@@ -3913,9 +4181,9 @@
       <c r="BV29" s="1"/>
       <c r="BW29" s="1"/>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>3008</v>
+    <row r="30" spans="1:75">
+      <c r="A30" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="1">
         <v>1.3031652217500001E-3</v>
@@ -4048,9 +4316,9 @@
       <c r="BV30" s="1"/>
       <c r="BW30" s="1"/>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>3010</v>
+    <row r="31" spans="1:75">
+      <c r="A31" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B31" s="1">
         <v>1.2974673048E-3</v>
@@ -4185,9 +4453,9 @@
       <c r="BV31" s="1"/>
       <c r="BW31" s="1"/>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>3012</v>
+    <row r="32" spans="1:75">
+      <c r="A32" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B32" s="1">
         <v>1.29614217413E-3</v>
@@ -4324,9 +4592,9 @@
       <c r="BV32" s="1"/>
       <c r="BW32" s="1"/>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>3014</v>
+    <row r="33" spans="1:75">
+      <c r="A33" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B33" s="1">
         <v>1.0590254299399999E-3</v>
@@ -4465,9 +4733,9 @@
       <c r="BV33" s="1"/>
       <c r="BW33" s="1"/>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>3016</v>
+    <row r="34" spans="1:75">
+      <c r="A34" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B34" s="1">
         <v>1.00789263291E-3</v>
@@ -4608,9 +4876,9 @@
       <c r="BV34" s="1"/>
       <c r="BW34" s="1"/>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>3020</v>
+    <row r="35" spans="1:75">
+      <c r="A35" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B35" s="1">
         <v>9.7737343748900002E-4</v>
@@ -4753,9 +5021,9 @@
       <c r="BV35" s="1"/>
       <c r="BW35" s="1"/>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>3022</v>
+    <row r="36" spans="1:75">
+      <c r="A36" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B36" s="1">
         <v>9.5466935601099998E-4</v>
@@ -4900,9 +5168,9 @@
       <c r="BV36" s="1"/>
       <c r="BW36" s="1"/>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>3030</v>
+    <row r="37" spans="1:75">
+      <c r="A37" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B37" s="1">
         <v>9.4358028413799998E-4</v>
@@ -5049,9 +5317,9 @@
       <c r="BV37" s="1"/>
       <c r="BW37" s="1"/>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>3034</v>
+    <row r="38" spans="1:75">
+      <c r="A38" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B38" s="1">
         <v>9.1735158119199997E-4</v>
@@ -5200,9 +5468,9 @@
       <c r="BV38" s="1"/>
       <c r="BW38" s="1"/>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>3040</v>
+    <row r="39" spans="1:75">
+      <c r="A39" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B39" s="1">
         <v>9.0179488518700001E-4</v>
@@ -5353,9 +5621,9 @@
       <c r="BV39" s="1"/>
       <c r="BW39" s="1"/>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>3042</v>
+    <row r="40" spans="1:75">
+      <c r="A40" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B40" s="1">
         <v>9.0472921873700003E-4</v>
@@ -5508,9 +5776,9 @@
       <c r="BV40" s="1"/>
       <c r="BW40" s="1"/>
     </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>3050</v>
+    <row r="41" spans="1:75">
+      <c r="A41" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B41" s="1">
         <v>8.4468518717199998E-4</v>
@@ -5665,9 +5933,9 @@
       <c r="BV41" s="1"/>
       <c r="BW41" s="1"/>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>3052</v>
+    <row r="42" spans="1:75">
+      <c r="A42" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B42" s="1">
         <v>8.5480957590299998E-4</v>
@@ -5824,9 +6092,9 @@
       <c r="BV42" s="1"/>
       <c r="BW42" s="1"/>
     </row>
-    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>3100</v>
+    <row r="43" spans="1:75">
+      <c r="A43" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B43" s="1">
         <v>7.7325993500900001E-4</v>
@@ -5985,9 +6253,9 @@
       <c r="BV43" s="1"/>
       <c r="BW43" s="1"/>
     </row>
-    <row r="44" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>3110</v>
+    <row r="44" spans="1:75">
+      <c r="A44" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B44" s="1">
         <v>7.8983033606700001E-4</v>
@@ -6148,9 +6416,9 @@
       <c r="BV44" s="1"/>
       <c r="BW44" s="1"/>
     </row>
-    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>4000</v>
+    <row r="45" spans="1:75">
+      <c r="A45" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B45" s="1">
         <v>7.5863030934499997E-4</v>
@@ -6313,9 +6581,9 @@
       <c r="BV45" s="1"/>
       <c r="BW45" s="1"/>
     </row>
-    <row r="46" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>4002</v>
+    <row r="46" spans="1:75">
+      <c r="A46" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B46" s="1">
         <v>7.4472024088099997E-4</v>
@@ -6480,9 +6748,9 @@
       <c r="BV46" s="1"/>
       <c r="BW46" s="1"/>
     </row>
-    <row r="47" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>4004</v>
+    <row r="47" spans="1:75">
+      <c r="A47" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B47" s="1">
         <v>7.4181395083399999E-4</v>
@@ -6649,9 +6917,9 @@
       <c r="BV47" s="1"/>
       <c r="BW47" s="1"/>
     </row>
-    <row r="48" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>4100</v>
+    <row r="48" spans="1:75">
+      <c r="A48" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B48" s="1">
         <v>7.2111543446500004E-4</v>
@@ -6820,9 +7088,9 @@
       <c r="BV48" s="1"/>
       <c r="BW48" s="1"/>
     </row>
-    <row r="49" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
-        <v>4102</v>
+    <row r="49" spans="1:75">
+      <c r="A49" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B49" s="1">
         <v>7.2065874760999995E-4</v>
@@ -6993,9 +7261,9 @@
       <c r="BV49" s="1"/>
       <c r="BW49" s="1"/>
     </row>
-    <row r="50" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>4104</v>
+    <row r="50" spans="1:75">
+      <c r="A50" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B50" s="1">
         <v>7.2036574933700005E-4</v>
@@ -7168,9 +7436,9 @@
       <c r="BV50" s="1"/>
       <c r="BW50" s="1"/>
     </row>
-    <row r="51" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>4200</v>
+    <row r="51" spans="1:75">
+      <c r="A51" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B51" s="1">
         <v>7.0538631924599998E-4</v>
@@ -7345,9 +7613,9 @@
       <c r="BV51" s="1"/>
       <c r="BW51" s="1"/>
     </row>
-    <row r="52" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>4202</v>
+    <row r="52" spans="1:75">
+      <c r="A52" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B52" s="1">
         <v>7.0128369449000004E-4</v>
@@ -7524,9 +7792,9 @@
       <c r="BV52" s="1"/>
       <c r="BW52" s="1"/>
     </row>
-    <row r="53" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>4204</v>
+    <row r="53" spans="1:75">
+      <c r="A53" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B53" s="1">
         <v>6.9371634884500002E-4</v>
@@ -7705,9 +7973,9 @@
       <c r="BV53" s="1"/>
       <c r="BW53" s="1"/>
     </row>
-    <row r="54" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>4208</v>
+    <row r="54" spans="1:75">
+      <c r="A54" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B54" s="1">
         <v>6.8062111833300004E-4</v>
@@ -7888,9 +8156,9 @@
       <c r="BV54" s="1"/>
       <c r="BW54" s="1"/>
     </row>
-    <row r="55" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
-        <v>4300</v>
+    <row r="55" spans="1:75">
+      <c r="A55" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B55" s="1">
         <v>6.2396846549400004E-4</v>
@@ -8073,9 +8341,9 @@
       <c r="BV55" s="1"/>
       <c r="BW55" s="1"/>
     </row>
-    <row r="56" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
-        <v>4302</v>
+    <row r="56" spans="1:75">
+      <c r="A56" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B56" s="1">
         <v>6.2378482418800002E-4</v>
@@ -8260,9 +8528,9 @@
       <c r="BV56" s="1"/>
       <c r="BW56" s="1"/>
     </row>
-    <row r="57" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
-        <v>4304</v>
+    <row r="57" spans="1:75">
+      <c r="A57" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B57" s="1">
         <v>6.2363701461400003E-4</v>
@@ -8449,9 +8717,9 @@
       <c r="BV57" s="1"/>
       <c r="BW57" s="1"/>
     </row>
-    <row r="58" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
-        <v>4306</v>
+    <row r="58" spans="1:75">
+      <c r="A58" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B58" s="1">
         <v>6.2552317374000004E-4</v>
@@ -8640,9 +8908,9 @@
       <c r="BV58" s="1"/>
       <c r="BW58" s="1"/>
     </row>
-    <row r="59" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
-        <v>4310</v>
+    <row r="59" spans="1:75">
+      <c r="A59" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B59" s="1">
         <v>6.1434042411300004E-4</v>
@@ -8833,9 +9101,9 @@
       <c r="BV59" s="1"/>
       <c r="BW59" s="1"/>
     </row>
-    <row r="60" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
-        <v>4312</v>
+    <row r="60" spans="1:75">
+      <c r="A60" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B60" s="1">
         <v>6.1366984818399999E-4</v>
@@ -9028,9 +9296,9 @@
       <c r="BV60" s="1"/>
       <c r="BW60" s="1"/>
     </row>
-    <row r="61" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
-        <v>4314</v>
+    <row r="61" spans="1:75">
+      <c r="A61" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B61" s="1">
         <v>6.1366984818399999E-4</v>
@@ -9225,9 +9493,9 @@
       <c r="BV61" s="1"/>
       <c r="BW61" s="1"/>
     </row>
-    <row r="62" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
-        <v>4400</v>
+    <row r="62" spans="1:75">
+      <c r="A62" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B62" s="1">
         <v>6.0924810643400002E-4</v>
@@ -9424,9 +9692,9 @@
       <c r="BV62" s="1"/>
       <c r="BW62" s="1"/>
     </row>
-    <row r="63" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
-        <v>4402</v>
+    <row r="63" spans="1:75">
+      <c r="A63" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B63" s="1">
         <v>6.0940157782800005E-4</v>
@@ -9625,9 +9893,9 @@
       <c r="BV63" s="1"/>
       <c r="BW63" s="1"/>
     </row>
-    <row r="64" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
-        <v>4404</v>
+    <row r="64" spans="1:75">
+      <c r="A64" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B64" s="1">
         <v>6.0933335877500004E-4</v>
@@ -9828,9 +10096,9 @@
       <c r="BV64" s="1"/>
       <c r="BW64" s="1"/>
     </row>
-    <row r="65" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
-        <v>4406</v>
+    <row r="65" spans="1:75">
+      <c r="A65" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B65" s="1">
         <v>6.0913808868000004E-4</v>
@@ -10033,9 +10301,9 @@
       <c r="BV65" s="1"/>
       <c r="BW65" s="1"/>
     </row>
-    <row r="66" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
-        <v>4410</v>
+    <row r="66" spans="1:75">
+      <c r="A66" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B66" s="1">
         <v>5.7145291904700003E-4</v>
@@ -10240,9 +10508,9 @@
       <c r="BV66" s="1"/>
       <c r="BW66" s="1"/>
     </row>
-    <row r="67" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
-        <v>4500</v>
+    <row r="67" spans="1:75">
+      <c r="A67" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B67" s="1">
         <v>5.7145721590100003E-4</v>
@@ -10449,9 +10717,9 @@
       <c r="BV67" s="1"/>
       <c r="BW67" s="1"/>
     </row>
-    <row r="68" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
-        <v>4502</v>
+    <row r="68" spans="1:75">
+      <c r="A68" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B68" s="1">
         <v>5.7135554102099998E-4</v>
@@ -10660,9 +10928,9 @@
       <c r="BV68" s="1"/>
       <c r="BW68" s="1"/>
     </row>
-    <row r="69" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
-        <v>4504</v>
+    <row r="69" spans="1:75">
+      <c r="A69" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B69" s="1">
         <v>5.70417831061E-4</v>
@@ -10873,9 +11141,9 @@
       <c r="BV69" s="1"/>
       <c r="BW69" s="1"/>
     </row>
-    <row r="70" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
-        <v>4510</v>
+    <row r="70" spans="1:75">
+      <c r="A70" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B70" s="1">
         <v>5.6856437495299999E-4</v>
@@ -11088,9 +11356,9 @@
       <c r="BV70" s="1"/>
       <c r="BW70" s="1"/>
     </row>
-    <row r="71" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
-        <v>4600</v>
+    <row r="71" spans="1:75">
+      <c r="A71" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B71" s="1">
         <v>5.9070687098399996E-4</v>
@@ -11305,9 +11573,9 @@
       <c r="BV71" s="1"/>
       <c r="BW71" s="1"/>
     </row>
-    <row r="72" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
-        <v>4602</v>
+    <row r="72" spans="1:75">
+      <c r="A72" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B72" s="1">
         <v>5.8895499915599995E-4</v>
@@ -11524,9 +11792,9 @@
       <c r="BV72" s="1"/>
       <c r="BW72" s="1"/>
     </row>
-    <row r="73" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
-        <v>4604</v>
+    <row r="73" spans="1:75">
+      <c r="A73" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B73" s="1">
         <v>5.8876928742900003E-4</v>
@@ -11745,9 +12013,9 @@
       <c r="BV73" s="1"/>
       <c r="BW73" s="1"/>
     </row>
-    <row r="74" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
-        <v>4700</v>
+    <row r="74" spans="1:75">
+      <c r="A74" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B74" s="1">
         <v>5.9594458463400001E-4</v>
@@ -11968,9 +12236,9 @@
       <c r="BV74" s="1"/>
       <c r="BW74" s="1"/>
     </row>
-    <row r="75" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
-        <v>4702</v>
+    <row r="75" spans="1:75">
+      <c r="A75" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B75" s="1">
         <v>5.9501951240800005E-4</v>
@@ -12193,9 +12461,9 @@
       </c>
       <c r="BW75" s="1"/>
     </row>
-    <row r="76" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
-        <v>4710</v>
+    <row r="76" spans="1:75">
+      <c r="A76" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B76" s="1">
         <v>5.8075254838600005E-4</v>
@@ -12420,232 +12688,233 @@
         <v>0.468706416982</v>
       </c>
     </row>
-    <row r="77" spans="1:75" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:75" s="3" customFormat="1" ht="39" customHeight="1">
       <c r="A77" s="2"/>
-      <c r="B77" s="2">
-        <v>2008</v>
-      </c>
-      <c r="C77" s="2">
-        <v>2010</v>
-      </c>
-      <c r="D77" s="2">
-        <v>2025</v>
-      </c>
-      <c r="E77" s="2">
-        <v>2026</v>
-      </c>
-      <c r="F77" s="2">
-        <v>2027</v>
-      </c>
-      <c r="G77" s="2">
-        <v>2030</v>
-      </c>
-      <c r="H77" s="2">
-        <v>2032</v>
-      </c>
-      <c r="I77" s="2">
-        <v>2040</v>
-      </c>
-      <c r="J77" s="2">
-        <v>2042</v>
-      </c>
-      <c r="K77" s="2">
-        <v>2060</v>
-      </c>
-      <c r="L77" s="2">
-        <v>2070</v>
-      </c>
-      <c r="M77" s="2">
-        <v>2080</v>
-      </c>
-      <c r="N77" s="2">
-        <v>2082</v>
-      </c>
-      <c r="O77" s="2">
-        <v>2084</v>
-      </c>
-      <c r="P77" s="2">
-        <v>2100</v>
-      </c>
-      <c r="Q77" s="2">
-        <v>2102</v>
-      </c>
-      <c r="R77" s="2">
-        <v>2104</v>
-      </c>
-      <c r="S77" s="2">
-        <v>2200</v>
-      </c>
-      <c r="T77" s="2">
-        <v>2202</v>
-      </c>
-      <c r="U77" s="2">
-        <v>2300</v>
-      </c>
-      <c r="V77" s="2">
-        <v>2302</v>
-      </c>
-      <c r="W77" s="2">
-        <v>2304</v>
-      </c>
-      <c r="X77" s="2">
-        <v>2306</v>
-      </c>
-      <c r="Y77" s="2">
-        <v>2400</v>
-      </c>
-      <c r="Z77" s="2">
-        <v>2402</v>
-      </c>
-      <c r="AA77" s="2">
-        <v>2500</v>
-      </c>
-      <c r="AB77" s="2">
-        <v>2502</v>
-      </c>
-      <c r="AC77" s="2">
-        <v>2504</v>
-      </c>
-      <c r="AD77" s="2">
-        <v>3006</v>
-      </c>
-      <c r="AE77" s="2">
-        <v>3008</v>
-      </c>
-      <c r="AF77" s="2">
-        <v>3010</v>
-      </c>
-      <c r="AG77" s="2">
-        <v>3012</v>
-      </c>
-      <c r="AH77" s="2">
-        <v>3014</v>
-      </c>
-      <c r="AI77" s="2">
-        <v>3016</v>
-      </c>
-      <c r="AJ77" s="2">
-        <v>3020</v>
-      </c>
-      <c r="AK77" s="2">
-        <v>3022</v>
-      </c>
-      <c r="AL77" s="2">
-        <v>3030</v>
-      </c>
-      <c r="AM77" s="2">
-        <v>3034</v>
-      </c>
-      <c r="AN77" s="2">
-        <v>3040</v>
-      </c>
-      <c r="AO77" s="2">
-        <v>3042</v>
-      </c>
-      <c r="AP77" s="2">
-        <v>3050</v>
-      </c>
-      <c r="AQ77" s="2">
-        <v>3052</v>
-      </c>
-      <c r="AR77" s="2">
-        <v>3100</v>
-      </c>
-      <c r="AS77" s="2">
-        <v>3110</v>
-      </c>
-      <c r="AT77" s="2">
-        <v>4000</v>
-      </c>
-      <c r="AU77" s="2">
-        <v>4002</v>
-      </c>
-      <c r="AV77" s="2">
-        <v>4004</v>
-      </c>
-      <c r="AW77" s="2">
-        <v>4100</v>
-      </c>
-      <c r="AX77" s="2">
-        <v>4102</v>
-      </c>
-      <c r="AY77" s="2">
-        <v>4104</v>
-      </c>
-      <c r="AZ77" s="2">
-        <v>4200</v>
-      </c>
-      <c r="BA77" s="2">
-        <v>4202</v>
-      </c>
-      <c r="BB77" s="2">
-        <v>4204</v>
-      </c>
-      <c r="BC77" s="2">
-        <v>4208</v>
-      </c>
-      <c r="BD77" s="2">
-        <v>4300</v>
-      </c>
-      <c r="BE77" s="2">
-        <v>4302</v>
-      </c>
-      <c r="BF77" s="2">
-        <v>4304</v>
-      </c>
-      <c r="BG77" s="2">
-        <v>4306</v>
-      </c>
-      <c r="BH77" s="2">
-        <v>4310</v>
-      </c>
-      <c r="BI77" s="2">
-        <v>4312</v>
-      </c>
-      <c r="BJ77" s="2">
-        <v>4314</v>
-      </c>
-      <c r="BK77" s="2">
-        <v>4400</v>
-      </c>
-      <c r="BL77" s="2">
-        <v>4402</v>
-      </c>
-      <c r="BM77" s="2">
-        <v>4404</v>
-      </c>
-      <c r="BN77" s="2">
-        <v>4406</v>
-      </c>
-      <c r="BO77" s="2">
-        <v>4410</v>
-      </c>
-      <c r="BP77" s="2">
-        <v>4500</v>
-      </c>
-      <c r="BQ77" s="2">
-        <v>4502</v>
-      </c>
-      <c r="BR77" s="2">
-        <v>4504</v>
-      </c>
-      <c r="BS77" s="2">
-        <v>4510</v>
-      </c>
-      <c r="BT77" s="2">
-        <v>4600</v>
-      </c>
-      <c r="BU77" s="2">
-        <v>4602</v>
-      </c>
-      <c r="BV77" s="2">
-        <v>4604</v>
-      </c>
-      <c r="BW77" s="2">
-        <v>4700</v>
+      <c r="B77" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T77" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U77" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V77" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W77" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y77" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z77" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA77" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC77" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD77" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE77" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF77" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG77" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH77" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI77" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ77" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK77" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL77" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM77" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN77" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO77" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP77" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS77" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT77" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU77" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV77" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW77" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY77" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ77" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="BA77" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="BB77" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BC77" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD77" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BE77" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF77" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BG77" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BH77" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BI77" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ77" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK77" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BL77" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM77" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BN77" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BO77" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BP77" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BQ77" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BR77" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BS77" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BT77" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BU77" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BV77" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BW77" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="B2:BW76">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -12659,6 +12928,14 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="41" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="38" orientation="portrait"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="75" max="1048575" man="1"/>
+  </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>